<commit_message>
fix: Correct number for death "other" OR, which should be same as val from April
</commit_message>
<xml_diff>
--- a/doc/June2020_new_comorbidity_OR.xlsx
+++ b/doc/June2020_new_comorbidity_OR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elipman\Repos\covid_risk_score\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902BF81C-79B1-46FA-94D1-EF97C3E228E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4009A2FC-BB27-4534-99FB-EFB53F539FD1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
+    <workbookView xWindow="10605" yWindow="-405" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
   </bookViews>
   <sheets>
     <sheet name="Data and methodology" sheetId="3" r:id="rId1"/>
@@ -281,7 +281,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,12 +304,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -395,9 +389,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -412,6 +403,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -912,7 +906,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,33 +916,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="16"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>62</v>
       </c>
       <c r="G2" t="s">
@@ -971,7 +965,7 @@
       <c r="F3">
         <v>6.11</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="20">
         <v>1.72</v>
       </c>
     </row>
@@ -991,7 +985,7 @@
       <c r="F4">
         <v>7.43</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="20">
         <v>1.27</v>
       </c>
     </row>
@@ -1011,7 +1005,7 @@
       <c r="F5">
         <v>4.7</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="20">
         <v>1.79</v>
       </c>
     </row>
@@ -1031,7 +1025,7 @@
       <c r="F6">
         <v>4.7</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1051,7 +1045,7 @@
       <c r="F7">
         <v>6.11</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="20">
         <v>1.1200000000000001</v>
       </c>
     </row>
@@ -1071,7 +1065,7 @@
       <c r="F8">
         <v>6.11</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <v>1.69</v>
       </c>
     </row>
@@ -1091,7 +1085,7 @@
       <c r="F9">
         <v>3.59</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="20">
         <v>1.78</v>
       </c>
     </row>
@@ -1111,12 +1105,12 @@
       <c r="F10">
         <v>6.11</v>
       </c>
-      <c r="G10" s="23">
-        <v>3.33</v>
+      <c r="G10" s="22">
+        <v>6.11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1443,7 +1437,7 @@
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>1.72</v>
       </c>
     </row>
@@ -1451,7 +1445,7 @@
       <c r="A6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>1.27</v>
       </c>
     </row>
@@ -1462,10 +1456,10 @@
       <c r="B7" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="20">
         <v>1.5</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="18">
         <v>1043176</v>
       </c>
     </row>
@@ -1473,10 +1467,10 @@
       <c r="B8" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="21">
         <v>2.36</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>489297</v>
       </c>
     </row>
@@ -1484,10 +1478,10 @@
       <c r="B9" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <v>1.87</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <v>195243</v>
       </c>
     </row>
@@ -1495,7 +1489,7 @@
       <c r="B10" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="19">
         <f>SUMPRODUCT(C7:C9,D7:D9)/SUM(D7:D9)</f>
         <v>1.7853682723317954</v>
       </c>
@@ -1504,7 +1498,7 @@
       <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="21">
         <v>0.95</v>
       </c>
     </row>
@@ -1515,10 +1509,10 @@
       <c r="B12" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="21">
         <v>1.25</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>5737545</v>
       </c>
     </row>
@@ -1526,10 +1520,10 @@
       <c r="B13" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <v>0.88</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>2962373</v>
       </c>
     </row>
@@ -1537,7 +1531,7 @@
       <c r="B14" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="19">
         <f>SUMPRODUCT(C12:C13,D12:D13)/SUM(D12:D13)</f>
         <v>1.1240128343738411</v>
       </c>
@@ -1546,7 +1540,7 @@
       <c r="A15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <v>1.69</v>
       </c>
     </row>
@@ -1554,7 +1548,7 @@
       <c r="A16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="19">
         <v>1.78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: Add OR for ICU obesity, which was missing before
</commit_message>
<xml_diff>
--- a/doc/June2020_new_comorbidity_OR.xlsx
+++ b/doc/June2020_new_comorbidity_OR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elipman\Repos\covid_risk_score\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EEB5FB-7C53-45C7-BB40-FFF33A42FD44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F60AF21-8BAE-4D59-9B46-42742F76723E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
   </bookViews>
   <sheets>
     <sheet name="Data and methodology" sheetId="3" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
   <si>
     <t>hospitalization</t>
   </si>
@@ -288,6 +288,9 @@
   <si>
     <t>NA</t>
   </si>
+  <si>
+    <t>ICU (from obesity study)</t>
+  </si>
 </sst>
 </file>
 
@@ -296,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +322,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -363,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -418,10 +427,13 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -758,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4884AB8-B5B9-4996-8D6E-379FBB0299BF}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3C4789-FE1E-4700-85D9-429D138DADB9}">
   <dimension ref="A1:XFD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,18 +945,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="22"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
@@ -1078,7 +1090,7 @@
       <c r="B8" s="13">
         <v>2.58</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="22">
         <v>2.58</v>
       </c>
       <c r="D8" s="13">
@@ -1099,7 +1111,7 @@
       <c r="B9" s="13">
         <v>2.5299999999999998</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="22">
         <v>1</v>
       </c>
       <c r="D9" s="13">
@@ -17518,7 +17530,7 @@
       <c r="B11" s="13">
         <v>4.21</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="22">
         <v>4.21</v>
       </c>
       <c r="D11" s="13">
@@ -17775,8 +17787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7307B198-172C-4241-84B1-7346FBD233A4}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17974,8 +17986,11 @@
       <c r="C16" s="18">
         <v>1.78</v>
       </c>
+      <c r="E16" s="11" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>66</v>
       </c>
@@ -17988,8 +18003,12 @@
       <c r="D17" s="17">
         <v>2404098</v>
       </c>
+      <c r="E17" s="24">
+        <f>(3.45/1.89)</f>
+        <v>1.8253968253968256</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>68</v>
       </c>
@@ -17999,8 +18018,12 @@
       <c r="D18" s="17">
         <v>929803</v>
       </c>
+      <c r="E18" s="24">
+        <f>7.36/1.69</f>
+        <v>4.3550295857988166</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>69</v>
       </c>
@@ -18010,8 +18033,12 @@
       <c r="D19" s="17">
         <v>466762</v>
       </c>
+      <c r="E19" s="24">
+        <f>7.36/1.69</f>
+        <v>4.3550295857988166</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>59</v>
       </c>
@@ -18019,8 +18046,12 @@
         <f>SUMPRODUCT(C17:C19,D17:D19)/SUM(D17:D19)</f>
         <v>1.4637569497742893</v>
       </c>
+      <c r="E20" s="18">
+        <f>SUMPRODUCT(E17:E19,D17:D19)/SUM(D17:D19)</f>
+        <v>2.7549179579020771</v>
+      </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>9</v>
       </c>
@@ -18028,7 +18059,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
fix: Update calculation of ICU obesity OR to be weighted average using n in obesity article rather than n from OpenSafely
</commit_message>
<xml_diff>
--- a/doc/June2020_new_comorbidity_OR.xlsx
+++ b/doc/June2020_new_comorbidity_OR.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elipman\Repos\covid_risk_score\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F60AF21-8BAE-4D59-9B46-42742F76723E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8E4827-8F8D-4869-9E50-F6512FF9947A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
   </bookViews>
   <sheets>
     <sheet name="Data and methodology" sheetId="3" r:id="rId1"/>
     <sheet name="Odds ratios for app" sheetId="1" r:id="rId2"/>
     <sheet name="Calc hospital ratios" sheetId="2" r:id="rId3"/>
-    <sheet name="Calc death ratios" sheetId="4" r:id="rId4"/>
+    <sheet name="Calc ICU rates (obesity only)" sheetId="5" r:id="rId4"/>
+    <sheet name="Calc death ratios" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
   <si>
     <t>hospitalization</t>
   </si>
@@ -289,7 +290,37 @@
     <t>NA</t>
   </si>
   <si>
-    <t>ICU (from obesity study)</t>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1002/oby.22831?af=R</t>
+  </si>
+  <si>
+    <t>April 202</t>
+  </si>
+  <si>
+    <t>Note very small sample size</t>
+  </si>
+  <si>
+    <t>BMI range</t>
+  </si>
+  <si>
+    <t>OR vs &lt;25</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>OR vs &lt;30 (obese vs. not obese)</t>
+  </si>
+  <si>
+    <t>25-30</t>
+  </si>
+  <si>
+    <t>30-35</t>
+  </si>
+  <si>
+    <t>&gt;35</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -372,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -430,12 +461,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -770,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4884AB8-B5B9-4996-8D6E-379FBB0299BF}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,25 +881,40 @@
       <c r="A11" t="s">
         <v>27</v>
       </c>
+      <c r="B11" s="25" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
+      <c r="B13" s="5">
+        <v>124</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
+      <c r="B14" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -925,6 +974,7 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" location="F1_down" display="https://www.cdc.gov/mmwr/volumes/69/wr/mm6925e1.htm?s_cid=mm6925e1_e&amp;deliveryName=USCDC_921-DM30747 - F1_down" xr:uid="{C4128523-1D22-4506-B540-6305E3743FC6}"/>
     <hyperlink ref="B19" r:id="rId2" xr:uid="{0A8EE84C-479D-4B3C-A99E-BD5E48C5E7E6}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{646A037C-CECB-45F6-9C6E-FD5168AD4163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -945,18 +995,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
@@ -17784,11 +17834,92 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7804BEA5-6FF4-4288-BCC9-5F2A2834F6D4}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="26">
+        <v>1.69</v>
+      </c>
+      <c r="D2" s="27"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="26">
+        <v>3.45</v>
+      </c>
+      <c r="D3" s="27">
+        <f>C3/$C$2</f>
+        <v>2.0414201183431953</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4">
+        <v>35</v>
+      </c>
+      <c r="C4" s="26">
+        <v>7.36</v>
+      </c>
+      <c r="D4" s="27">
+        <f>C4/$C$2</f>
+        <v>4.3550295857988166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="27">
+        <f>SUMPRODUCT(B3:B4,D3:D4)/SUM(B3:B4)</f>
+        <v>3.4139003109016146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7307B198-172C-4241-84B1-7346FBD233A4}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17986,9 +18117,7 @@
       <c r="C16" s="18">
         <v>1.78</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>71</v>
-      </c>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
@@ -18003,10 +18132,7 @@
       <c r="D17" s="17">
         <v>2404098</v>
       </c>
-      <c r="E17" s="24">
-        <f>(3.45/1.89)</f>
-        <v>1.8253968253968256</v>
-      </c>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
@@ -18018,10 +18144,7 @@
       <c r="D18" s="17">
         <v>929803</v>
       </c>
-      <c r="E18" s="24">
-        <f>7.36/1.69</f>
-        <v>4.3550295857988166</v>
-      </c>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
@@ -18033,10 +18156,7 @@
       <c r="D19" s="17">
         <v>466762</v>
       </c>
-      <c r="E19" s="24">
-        <f>7.36/1.69</f>
-        <v>4.3550295857988166</v>
-      </c>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
@@ -18046,10 +18166,7 @@
         <f>SUMPRODUCT(C17:C19,D17:D19)/SUM(D17:D19)</f>
         <v>1.4637569497742893</v>
       </c>
-      <c r="E20" s="18">
-        <f>SUMPRODUCT(E17:E19,D17:D19)/SUM(D17:D19)</f>
-        <v>2.7549179579020771</v>
-      </c>
+      <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">

</xml_diff>

<commit_message>
fix: Add obesity ICU number to main tab (from ICU tab)
</commit_message>
<xml_diff>
--- a/doc/June2020_new_comorbidity_OR.xlsx
+++ b/doc/June2020_new_comorbidity_OR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elipman\Repos\covid_risk_score\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8E4827-8F8D-4869-9E50-F6512FF9947A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68271938-1002-4BB3-A9EB-D8915036C1ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
   </bookViews>
   <sheets>
     <sheet name="Data and methodology" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t>hospitalization</t>
   </si>
@@ -464,12 +464,12 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -881,7 +881,7 @@
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>71</v>
       </c>
     </row>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3C4789-FE1E-4700-85D9-429D138DADB9}">
   <dimension ref="A1:XFD36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,18 +995,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
@@ -1185,10 +1185,10 @@
       <c r="C10" s="19">
         <v>1.9</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="19"/>
+      <c r="D10" s="19">
+        <v>3.41</v>
+      </c>
+      <c r="E10" s="20"/>
       <c r="F10" s="19" t="s">
         <v>70</v>
       </c>
@@ -17837,8 +17837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7804BEA5-6FF4-4288-BCC9-5F2A2834F6D4}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17856,7 +17856,7 @@
       <c r="C1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>77</v>
       </c>
     </row>
@@ -17864,10 +17864,10 @@
       <c r="A2" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="25">
         <v>1.69</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -17876,10 +17876,10 @@
       <c r="B3">
         <v>24</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>3.45</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="26">
         <f>C3/$C$2</f>
         <v>2.0414201183431953</v>
       </c>
@@ -17891,10 +17891,10 @@
       <c r="B4">
         <v>35</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="25">
         <v>7.36</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <f>C4/$C$2</f>
         <v>4.3550295857988166</v>
       </c>
@@ -17903,7 +17903,7 @@
       <c r="A5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <f>SUMPRODUCT(B3:B4,D3:D4)/SUM(B3:B4)</f>
         <v>3.4139003109016146</v>
       </c>

</xml_diff>

<commit_message>
feat: implement conditional probability of ICU given hosp to fix ICU risk
</commit_message>
<xml_diff>
--- a/doc/June2020_new_comorbidity_OR.xlsx
+++ b/doc/June2020_new_comorbidity_OR.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elipman\Repos\covid_risk_score\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHu\OneDrive - Mathematica\Desktop\COVID19_hackathon\covid_risk_score\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68271938-1002-4BB3-A9EB-D8915036C1ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{68271938-1002-4BB3-A9EB-D8915036C1ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A91E069B-8D33-4C7F-9197-99BD38BA0F95}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
+    <workbookView xWindow="60" yWindow="-24120" windowWidth="38640" windowHeight="23640" activeTab="4" xr2:uid="{F2E07857-7E52-41DE-9EE1-01627E19B126}"/>
   </bookViews>
   <sheets>
     <sheet name="Data and methodology" sheetId="3" r:id="rId1"/>
     <sheet name="Odds ratios for app" sheetId="1" r:id="rId2"/>
     <sheet name="Calc hospital ratios" sheetId="2" r:id="rId3"/>
     <sheet name="Calc ICU rates (obesity only)" sheetId="5" r:id="rId4"/>
-    <sheet name="Calc death ratios" sheetId="4" r:id="rId5"/>
+    <sheet name="Calc Prob(ICU|hosp)" sheetId="6" r:id="rId5"/>
+    <sheet name="Calc death ratios" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
     <author>tc={E419212A-5901-437F-ADCB-180CABA12709}</author>
   </authors>
   <commentList>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{C38A0EDC-4FB0-4685-A489-4DB24ADD9BD0}">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{C38A0EDC-4FB0-4685-A489-4DB24ADD9BD0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="126">
   <si>
     <t>hospitalization</t>
   </si>
@@ -256,9 +257,6 @@
     <t>June</t>
   </si>
   <si>
-    <t>Cases where OR is not directly from literature are highlighted</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Outcome is risk of death in entire population, </t>
     </r>
@@ -322,6 +320,190 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>Cases where OR is not mutually adjusted for other demographic characteristics are highlighted in green</t>
+  </si>
+  <si>
+    <t>Cases where OR is not directly from literature are highlighted in yellow</t>
+  </si>
+  <si>
+    <t>Comorbidity</t>
+  </si>
+  <si>
+    <t>Hospitalized, non-ICU</t>
+  </si>
+  <si>
+    <t>ICU admission</t>
+  </si>
+  <si>
+    <t>P(ICU | hosp)</t>
+  </si>
+  <si>
+    <t>Diabetes mellitus (784, 10.9%)</t>
+  </si>
+  <si>
+    <t>251 (24)</t>
+  </si>
+  <si>
+    <t>148 (32)</t>
+  </si>
+  <si>
+    <t>Chronic lung disease* (656, 9.2%)</t>
+  </si>
+  <si>
+    <t>152 (15)</t>
+  </si>
+  <si>
+    <t>94 (21)</t>
+  </si>
+  <si>
+    <t>Cardiovascular disease (647, 9.0%)</t>
+  </si>
+  <si>
+    <t>242 (23)</t>
+  </si>
+  <si>
+    <t>132 (29)</t>
+  </si>
+  <si>
+    <t>Immunocompromised condition (264, 3.7%)</t>
+  </si>
+  <si>
+    <t>63 (6)</t>
+  </si>
+  <si>
+    <t>41 (9)</t>
+  </si>
+  <si>
+    <t>Chronic renal disease (213, 3.0%)</t>
+  </si>
+  <si>
+    <t>95 (9)</t>
+  </si>
+  <si>
+    <t>56 (12)</t>
+  </si>
+  <si>
+    <t>Pregnancy (143, 2.0%)</t>
+  </si>
+  <si>
+    <t>31 (3)</t>
+  </si>
+  <si>
+    <t>4 (1)</t>
+  </si>
+  <si>
+    <r>
+      <t>Neurologic disorder, neurodevelopmental, intellectual disability (52, 0.7%)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>†</t>
+    </r>
+  </si>
+  <si>
+    <t>25 (2)</t>
+  </si>
+  <si>
+    <t>7 (2)</t>
+  </si>
+  <si>
+    <t>Chronic liver disease (41, 0.6%)</t>
+  </si>
+  <si>
+    <t>9 (1)</t>
+  </si>
+  <si>
+    <r>
+      <t>Other chronic disease (1,182, 16.5%)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>§</t>
+    </r>
+  </si>
+  <si>
+    <t>359 (35)</t>
+  </si>
+  <si>
+    <t>170 (37)</t>
+  </si>
+  <si>
+    <t>Former smoker (165, 2.3%)</t>
+  </si>
+  <si>
+    <t>45 (4)</t>
+  </si>
+  <si>
+    <t>33 (7)</t>
+  </si>
+  <si>
+    <t>Current smoker (96, 1.3%)</t>
+  </si>
+  <si>
+    <t>22 (2)</t>
+  </si>
+  <si>
+    <t>5 (1)</t>
+  </si>
+  <si>
+    <r>
+      <t>None of the above conditions</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>¶</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (4,470, 62.4%)</t>
+    </r>
+  </si>
+  <si>
+    <t>305 (29)</t>
+  </si>
+  <si>
+    <t>99 (22)</t>
+  </si>
+  <si>
+    <t>Table 1 in CDC MMWR 69(13) https://www.cdc.gov/mmwr/volumes/69/wr/mm6913e2.htm?s_cid=mm6913e2_w</t>
+  </si>
+  <si>
+    <t>Ever smoker (165+96 = 261)</t>
+  </si>
 </sst>
 </file>
 
@@ -330,7 +512,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,8 +542,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +577,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,11 +611,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -470,10 +683,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -791,7 +1025,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G6" dT="2020-06-23T21:31:55.87" personId="{8D3E2C0F-4A3B-4698-B547-21D7821E0DE5}" id="{C38A0EDC-4FB0-4685-A489-4DB24ADD9BD0}">
+  <threadedComment ref="I6" dT="2020-06-23T21:31:55.87" personId="{8D3E2C0F-4A3B-4698-B547-21D7821E0DE5}" id="{C38A0EDC-4FB0-4685-A489-4DB24ADD9BD0}">
     <text>Brought up to 1 from .95</text>
   </threadedComment>
   <threadedComment ref="C9" dT="2020-06-23T21:16:18.73" personId="{8D3E2C0F-4A3B-4698-B547-21D7821E0DE5}" id="{E419212A-5901-437F-ADCB-180CABA12709}">
@@ -804,22 +1038,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4884AB8-B5B9-4996-8D6E-379FBB0299BF}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -827,7 +1061,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -835,7 +1069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -843,7 +1077,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -851,7 +1085,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -859,7 +1093,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -867,33 +1101,33 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -901,7 +1135,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -909,20 +1143,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -930,7 +1164,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -938,7 +1172,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -946,7 +1180,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -954,7 +1188,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -962,12 +1196,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -984,51 +1218,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3C4789-FE1E-4700-85D9-429D138DADB9}">
   <dimension ref="A1:XFD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="27"/>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="B2" s="15" t="s">
         <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>63</v>
       </c>
+      <c r="J2" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1038,18 +1284,29 @@
       <c r="C3" s="13">
         <v>2.6</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="31">
         <v>5.82</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13">
+      <c r="F3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="13">
         <v>6.11</v>
       </c>
-      <c r="G3" s="19">
+      <c r="I3" s="19">
         <v>1.72</v>
       </c>
+      <c r="J3" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1059,18 +1316,29 @@
       <c r="C4" s="13">
         <v>1.4</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="31">
         <v>4.88</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13">
+      <c r="F4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="13">
         <v>7.43</v>
       </c>
-      <c r="G4" s="19">
+      <c r="I4" s="19">
         <v>1.27</v>
       </c>
+      <c r="J4" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1080,18 +1348,29 @@
       <c r="C5" s="13">
         <v>3.1</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="13">
         <v>4.57</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13">
+      <c r="F5" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1.6</v>
+      </c>
+      <c r="H5" s="13">
         <v>4.7</v>
       </c>
-      <c r="G5" s="19">
+      <c r="I5" s="19">
         <v>1.79</v>
       </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1101,18 +1380,29 @@
       <c r="C6" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="13">
         <v>4.57</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13">
+      <c r="F6" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="13">
+        <v>2.29</v>
+      </c>
+      <c r="H6" s="13">
         <v>4.7</v>
       </c>
-      <c r="G6" s="21">
+      <c r="I6" s="21">
         <v>1</v>
       </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1122,39 +1412,61 @@
       <c r="C7" s="13">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="31">
         <v>2.64</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13">
+      <c r="F7" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="13">
         <v>6.11</v>
       </c>
-      <c r="G7" s="19">
+      <c r="I7" s="19">
         <v>1.1200000000000001</v>
       </c>
+      <c r="J7" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="13">
         <v>2.58</v>
       </c>
-      <c r="C8" s="22">
-        <v>2.58</v>
-      </c>
-      <c r="D8" s="13">
+      <c r="C8" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="31">
         <v>2.86</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13">
+      <c r="F8" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="13">
         <v>6.11</v>
       </c>
-      <c r="G8" s="19">
+      <c r="I8" s="19">
         <v>1.69</v>
       </c>
+      <c r="J8" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1164,40 +1476,59 @@
       <c r="C9" s="22">
         <v>1</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="31">
         <v>2.83</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13">
+      <c r="F9" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="13">
         <v>3.59</v>
       </c>
-      <c r="G9" s="19">
+      <c r="I9" s="19">
         <v>1.78</v>
       </c>
+      <c r="J9" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="19">
         <v>1.9</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="19">
         <v>3.41</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="19">
+      <c r="F10" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="19">
         <v>1.46</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="J10" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
@@ -17573,38 +17904,54 @@
       <c r="XFC10" s="18"/>
       <c r="XFD10" s="18"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="22">
         <v>4.21</v>
       </c>
-      <c r="C11" s="22">
-        <v>4.21</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="C11" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="22">
         <v>3.33</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13">
+      <c r="F11" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="22">
         <v>6.11</v>
       </c>
-      <c r="G11" s="21">
-        <v>6.11</v>
+      <c r="I11" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="36" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.35">
+      <c r="A14" s="30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" ht="42" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17617,16 +17964,16 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -17646,7 +17993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -17669,7 +18016,7 @@
         <v>4.4543117890372991E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -17686,7 +18033,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -17709,7 +18056,7 @@
         <v>3.961607714223328E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -17726,7 +18073,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -17743,7 +18090,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -17760,7 +18107,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -17777,7 +18124,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -17794,7 +18141,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -17811,7 +18158,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -17841,37 +18188,37 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="26" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
       </c>
       <c r="C2" s="25">
         <v>1.69</v>
       </c>
       <c r="D2" s="26"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>24</v>
@@ -17884,9 +18231,9 @@
         <v>2.0414201183431953</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4">
         <v>35</v>
@@ -17899,9 +18246,9 @@
         <v>4.3550295857988166</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="26">
         <f>SUMPRODUCT(B3:B4,D3:D4)/SUM(B3:B4)</f>
@@ -17915,27 +18262,257 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DC60E6-39C8-4521-8F2D-426955DC2738}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="22.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="35">
+        <f>148/(148+251)</f>
+        <v>0.37092731829573933</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="35">
+        <f>94/(94+152)</f>
+        <v>0.38211382113821141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="35">
+        <f>132/(132+242)</f>
+        <v>0.35294117647058826</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="35">
+        <f>41/(41+63)</f>
+        <v>0.39423076923076922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="35">
+        <f>56/(56+95)</f>
+        <v>0.37086092715231789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="35">
+        <f>4/(4+31)</f>
+        <v>0.11428571428571428</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.35">
+      <c r="A9" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="35">
+        <f>7/(7+25)</f>
+        <v>0.21875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="35">
+        <f>7/(7+9)</f>
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="35">
+        <f>170/(170+359)</f>
+        <v>0.32136105860113423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="35">
+        <f>33/(33+45)</f>
+        <v>0.42307692307692307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="35">
+        <f>5/(5+22)</f>
+        <v>0.18518518518518517</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="33">
+        <v>67</v>
+      </c>
+      <c r="C14" s="33">
+        <v>38</v>
+      </c>
+      <c r="D14" s="35">
+        <f>C14/(C14+B14)</f>
+        <v>0.3619047619047619</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="35">
+        <f>99/(99+305)</f>
+        <v>0.24504950495049505</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7307B198-172C-4241-84B1-7346FBD233A4}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="13"/>
-    <col min="5" max="5" width="21.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.26953125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="13"/>
+    <col min="5" max="5" width="21.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="23.26953125" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="13"/>
+    <col min="9" max="16384" width="9.1796875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>43</v>
       </c>
@@ -17958,7 +18535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="13">
         <v>1.38E-2</v>
       </c>
@@ -17985,7 +18562,7 @@
         <v>1.38E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>50</v>
       </c>
@@ -17999,7 +18576,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
@@ -18007,7 +18584,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
@@ -18015,7 +18592,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
@@ -18029,7 +18606,7 @@
         <v>1043176</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>55</v>
       </c>
@@ -18040,7 +18617,7 @@
         <v>489297</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>56</v>
       </c>
@@ -18051,7 +18628,7 @@
         <v>195243</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="13" t="s">
         <v>57</v>
       </c>
@@ -18060,7 +18637,7 @@
         <v>1.7853682723317954</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
@@ -18068,7 +18645,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>7</v>
       </c>
@@ -18082,7 +18659,7 @@
         <v>5737545</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" s="13" t="s">
         <v>60</v>
       </c>
@@ -18093,7 +18670,7 @@
         <v>2962373</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" s="13" t="s">
         <v>59</v>
       </c>
@@ -18102,7 +18679,7 @@
         <v>1.1240128343738411</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>11</v>
       </c>
@@ -18110,7 +18687,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>8</v>
       </c>
@@ -18119,12 +18696,12 @@
       </c>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>66</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>67</v>
       </c>
       <c r="C17" s="18">
         <v>1.27</v>
@@ -18134,9 +18711,9 @@
       </c>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B18" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="18">
         <v>1.56</v>
@@ -18146,9 +18723,9 @@
       </c>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="18">
         <v>2.27</v>
@@ -18158,7 +18735,7 @@
       </c>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" s="13" t="s">
         <v>59</v>
       </c>
@@ -18168,7 +18745,7 @@
       </c>
       <c r="E20" s="18"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>9</v>
       </c>
@@ -18176,7 +18753,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>49</v>
       </c>

</xml_diff>